<commit_message>
advanced stats - wrs
</commit_message>
<xml_diff>
--- a/wr_stats/cfb_2019_wr.xlsx
+++ b/wr_stats/cfb_2019_wr.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5148b8ebb4ef3d6a/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akulk\PycharmProjects\nflmetrics\wr_stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B2153E3-388C-47F5-9F68-21C9D1ACA1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63938405-BC21-42F1-9100-DB83B7FC24F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1875" yWindow="-120" windowWidth="18735" windowHeight="11760" xr2:uid="{62CE4C00-4FF1-40D6-83CD-E68C76B467EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$201</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1351,8 +1354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBAB0F96-F96D-47F1-BD93-10D5C29A0CD4}">
   <dimension ref="A1:I201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
+      <selection activeCell="I202" sqref="I202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7185,8 +7188,12 @@
       <c r="H201">
         <v>17</v>
       </c>
+      <c r="I201">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I201" xr:uid="{CBAB0F96-F96D-47F1-BD93-10D5C29A0CD4}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>